<commit_message>
mma seagrass graphs to match jumby additions
</commit_message>
<xml_diff>
--- a/mma/data/mma_seagrass.xlsx
+++ b/mma/data/mma_seagrass.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="quadrants" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="quadrats" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="site description" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="inverts" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="lookups" sheetId="4" r:id="rId7"/>
@@ -44,7 +44,7 @@
     <t>transect</t>
   </si>
   <si>
-    <t>quadrant</t>
+    <t>quadrat</t>
   </si>
   <si>
     <t>code</t>
@@ -350,6 +350,9 @@
     <t>Halophila stipulacea</t>
   </si>
   <si>
+    <t>Invasive seagrass</t>
+  </si>
+  <si>
     <t>HAL</t>
   </si>
   <si>
@@ -455,7 +458,7 @@
     <t>Sponge</t>
   </si>
   <si>
-    <t>Sponges, tunicates &amp; soft coral</t>
+    <t>Sponges, tunicates &amp; corals</t>
   </si>
   <si>
     <t>GOR</t>
@@ -468,9 +471,6 @@
   </si>
   <si>
     <t>Porites divaricata</t>
-  </si>
-  <si>
-    <t>Stony coral</t>
   </si>
   <si>
     <t>PPOR</t>
@@ -509,6 +509,18 @@
     <t>Manicina areolata</t>
   </si>
   <si>
+    <t>CARB</t>
+  </si>
+  <si>
+    <t>Cladocora arbuscula</t>
+  </si>
+  <si>
+    <t>TUN</t>
+  </si>
+  <si>
+    <t>Tunicate</t>
+  </si>
+  <si>
     <t>ANE</t>
   </si>
   <si>
@@ -540,18 +552,6 @@
   </si>
   <si>
     <t>Macrodactyla doreensis</t>
-  </si>
-  <si>
-    <t>CARB</t>
-  </si>
-  <si>
-    <t>Cladocora arbuscula</t>
-  </si>
-  <si>
-    <t>TUN</t>
-  </si>
-  <si>
-    <t>Tunicate</t>
   </si>
   <si>
     <t>CYAN</t>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="I75" s="6" t="str">
         <f>VLOOKUP(F75,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="76">
@@ -3335,7 +3335,7 @@
       </c>
       <c r="I77" s="6" t="str">
         <f>VLOOKUP(F77,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="78">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="I79" s="6" t="str">
         <f>VLOOKUP(F79,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="80">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="I81" s="6" t="str">
         <f>VLOOKUP(F81,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="82">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="I83" s="6" t="str">
         <f>VLOOKUP(F83,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="84">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="I85" s="6" t="str">
         <f>VLOOKUP(F85,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="86">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="I87" s="6" t="str">
         <f>VLOOKUP(F87,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="88">
@@ -3738,7 +3738,7 @@
       </c>
       <c r="I90" s="6" t="str">
         <f>VLOOKUP(F90,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="91">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="I93" s="6" t="str">
         <f>VLOOKUP(F93,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="94">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="I97" s="6" t="str">
         <f>VLOOKUP(F97,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="98">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="I100" s="6" t="str">
         <f>VLOOKUP(F100,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="101">
@@ -4110,7 +4110,7 @@
       </c>
       <c r="I102" s="6" t="str">
         <f>VLOOKUP(F102,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="103">
@@ -4172,7 +4172,7 @@
       </c>
       <c r="I104" s="6" t="str">
         <f>VLOOKUP(F104,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="105">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="I106" s="6" t="str">
         <f>VLOOKUP(F106,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="107">
@@ -4296,7 +4296,7 @@
       </c>
       <c r="I108" s="6" t="str">
         <f>VLOOKUP(F108,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="109">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="I110" s="6" t="str">
         <f>VLOOKUP(F110,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="111">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="I112" s="6" t="str">
         <f>VLOOKUP(F112,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="113">
@@ -4482,7 +4482,7 @@
       </c>
       <c r="I114" s="6" t="str">
         <f>VLOOKUP(F114,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="115">
@@ -4544,7 +4544,7 @@
       </c>
       <c r="I116" s="6" t="str">
         <f>VLOOKUP(F116,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="117">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="I118" s="6" t="str">
         <f>VLOOKUP(F118,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="119">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="I133" s="6" t="str">
         <f>VLOOKUP(F133,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="134">
@@ -6311,7 +6311,7 @@
       </c>
       <c r="I173" s="6" t="str">
         <f>VLOOKUP(F173,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="174">
@@ -13503,7 +13503,7 @@
       </c>
       <c r="I405" s="6" t="str">
         <f>VLOOKUP(F405,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="406">
@@ -13627,7 +13627,7 @@
       </c>
       <c r="I409" s="6" t="str">
         <f>VLOOKUP(F409,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="410">
@@ -13813,7 +13813,7 @@
       </c>
       <c r="I415" s="6" t="str">
         <f>VLOOKUP(F415,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="416">
@@ -13999,7 +13999,7 @@
       </c>
       <c r="I421" s="6" t="str">
         <f>VLOOKUP(F421,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="422">
@@ -14464,7 +14464,7 @@
       </c>
       <c r="I436" s="6" t="str">
         <f>VLOOKUP(F436,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="437">
@@ -14619,7 +14619,7 @@
       </c>
       <c r="I441" s="6" t="str">
         <f>VLOOKUP(F441,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="442">
@@ -14650,7 +14650,7 @@
       </c>
       <c r="I442" s="6" t="str">
         <f>VLOOKUP(F442,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="443">
@@ -15146,7 +15146,7 @@
       </c>
       <c r="I458" s="6" t="str">
         <f>VLOOKUP(F458,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="459">
@@ -15239,7 +15239,7 @@
       </c>
       <c r="I461" s="6" t="str">
         <f>VLOOKUP(F461,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="462">
@@ -15270,7 +15270,7 @@
       </c>
       <c r="I462" s="6" t="str">
         <f>VLOOKUP(F462,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="463">
@@ -15487,7 +15487,7 @@
       </c>
       <c r="I469" s="6" t="str">
         <f>VLOOKUP(F469,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="470">
@@ -15735,7 +15735,7 @@
       </c>
       <c r="I477" s="6" t="str">
         <f>VLOOKUP(F477,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="478">
@@ -15797,7 +15797,7 @@
       </c>
       <c r="I479" s="6" t="str">
         <f>VLOOKUP(F479,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="480">
@@ -16324,7 +16324,7 @@
       </c>
       <c r="I496" s="6" t="str">
         <f>VLOOKUP(F496,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="497">
@@ -16541,7 +16541,7 @@
       </c>
       <c r="I503" s="6" t="str">
         <f>VLOOKUP(F503,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="504">
@@ -16820,7 +16820,7 @@
       </c>
       <c r="I512" s="6" t="str">
         <f>VLOOKUP(F512,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="513">
@@ -16944,7 +16944,7 @@
       </c>
       <c r="I516" s="6" t="str">
         <f>VLOOKUP(F516,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="517">
@@ -17161,7 +17161,7 @@
       </c>
       <c r="I523" s="6" t="str">
         <f>VLOOKUP(F523,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="524">
@@ -17378,7 +17378,7 @@
       </c>
       <c r="I530" s="6" t="str">
         <f>VLOOKUP(F530,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="531">
@@ -17440,7 +17440,7 @@
       </c>
       <c r="I532" s="6" t="str">
         <f>VLOOKUP(F532,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="533">
@@ -17502,7 +17502,7 @@
       </c>
       <c r="I534" s="6" t="str">
         <f>VLOOKUP(F534,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="535">
@@ -17564,7 +17564,7 @@
       </c>
       <c r="I536" s="6" t="str">
         <f>VLOOKUP(F536,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="537">
@@ -17719,7 +17719,7 @@
       </c>
       <c r="I541" s="6" t="str">
         <f>VLOOKUP(F541,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="542">
@@ -17874,7 +17874,7 @@
       </c>
       <c r="I546" s="6" t="str">
         <f>VLOOKUP(F546,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="547">
@@ -17936,7 +17936,7 @@
       </c>
       <c r="I548" s="6" t="str">
         <f>VLOOKUP(F548,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="549">
@@ -17967,7 +17967,7 @@
       </c>
       <c r="I549" s="6" t="str">
         <f>VLOOKUP(F549,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="550">
@@ -18122,7 +18122,7 @@
       </c>
       <c r="I554" s="6" t="str">
         <f>VLOOKUP(F554,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="555">
@@ -18277,7 +18277,7 @@
       </c>
       <c r="I559" s="6" t="str">
         <f>VLOOKUP(F559,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="560">
@@ -18308,7 +18308,7 @@
       </c>
       <c r="I560" s="6" t="str">
         <f>VLOOKUP(F560,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="561">
@@ -18494,7 +18494,7 @@
       </c>
       <c r="I566" s="6" t="str">
         <f>VLOOKUP(F566,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="567">
@@ -18556,7 +18556,7 @@
       </c>
       <c r="I568" s="6" t="str">
         <f>VLOOKUP(F568,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="569">
@@ -18680,7 +18680,7 @@
       </c>
       <c r="I572" s="6" t="str">
         <f>VLOOKUP(F572,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="573">
@@ -18804,7 +18804,7 @@
       </c>
       <c r="I576" s="6" t="str">
         <f>VLOOKUP(F576,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="577">
@@ -18835,7 +18835,7 @@
       </c>
       <c r="I577" s="6" t="str">
         <f>VLOOKUP(F577,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="578">
@@ -18866,7 +18866,7 @@
       </c>
       <c r="I578" s="6" t="str">
         <f>VLOOKUP(F578,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="579">
@@ -19083,7 +19083,7 @@
       </c>
       <c r="I585" s="6" t="str">
         <f>VLOOKUP(F585,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="586">
@@ -19176,7 +19176,7 @@
       </c>
       <c r="I588" s="6" t="str">
         <f>VLOOKUP(F588,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="589">
@@ -19362,7 +19362,7 @@
       </c>
       <c r="I594" s="6" t="str">
         <f>VLOOKUP(F594,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="595">
@@ -19610,7 +19610,7 @@
       </c>
       <c r="I602" s="6" t="str">
         <f>VLOOKUP(F602,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="603">
@@ -19672,7 +19672,7 @@
       </c>
       <c r="I604" s="6" t="str">
         <f>VLOOKUP(F604,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="605">
@@ -19765,7 +19765,7 @@
       </c>
       <c r="I607" s="6" t="str">
         <f>VLOOKUP(F607,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="608">
@@ -19858,7 +19858,7 @@
       </c>
       <c r="I610" s="6" t="str">
         <f>VLOOKUP(F610,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="611">
@@ -23051,7 +23051,7 @@
       </c>
       <c r="I713" s="6" t="str">
         <f>VLOOKUP(F713,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="714">
@@ -23082,7 +23082,7 @@
       </c>
       <c r="I714" s="6" t="str">
         <f>VLOOKUP(F714,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="715">
@@ -23578,7 +23578,7 @@
       </c>
       <c r="I730" s="6" t="str">
         <f>VLOOKUP(F730,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="731">
@@ -23919,7 +23919,7 @@
       </c>
       <c r="I741" s="6" t="str">
         <f>VLOOKUP(F741,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="742">
@@ -24539,7 +24539,7 @@
       </c>
       <c r="I761" s="6" t="str">
         <f>VLOOKUP(F761,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="762">
@@ -24973,7 +24973,7 @@
       </c>
       <c r="I775" s="6" t="str">
         <f>VLOOKUP(F775,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="776">
@@ -25779,7 +25779,7 @@
       </c>
       <c r="I801" s="6" t="str">
         <f>VLOOKUP(F801,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="802">
@@ -26337,7 +26337,7 @@
       </c>
       <c r="I819" s="6" t="str">
         <f>VLOOKUP(F819,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="820">
@@ -26802,7 +26802,7 @@
       </c>
       <c r="I834" s="6" t="str">
         <f>VLOOKUP(F834,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="835">
@@ -26957,7 +26957,7 @@
       </c>
       <c r="I839" s="6" t="str">
         <f>VLOOKUP(F839,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="840">
@@ -27453,7 +27453,7 @@
       </c>
       <c r="I855" s="6" t="str">
         <f>VLOOKUP(F855,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="856">
@@ -28972,7 +28972,7 @@
       </c>
       <c r="I904" s="6" t="str">
         <f>VLOOKUP(F904,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="905">
@@ -29592,7 +29592,7 @@
       </c>
       <c r="I924" s="6" t="str">
         <f>VLOOKUP(F924,lookups!$2:$110,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="925">
@@ -31204,7 +31204,7 @@
       </c>
       <c r="I976" s="6" t="str">
         <f>VLOOKUP(F976,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="977">
@@ -31793,7 +31793,7 @@
       </c>
       <c r="I995" s="6" t="str">
         <f>VLOOKUP(F995,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="996">
@@ -33467,7 +33467,7 @@
       </c>
       <c r="I1049" s="6" t="str">
         <f>VLOOKUP(F1049,lookups!$2:$110,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1050">
@@ -33994,7 +33994,7 @@
       </c>
       <c r="I1066" s="6" t="str">
         <f>VLOOKUP(F1066,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1067">
@@ -34118,7 +34118,7 @@
       </c>
       <c r="I1070" s="6" t="str">
         <f>VLOOKUP(F1070,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1071">
@@ -34242,7 +34242,7 @@
       </c>
       <c r="I1074" s="6" t="str">
         <f>VLOOKUP(F1074,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1075">
@@ -34366,7 +34366,7 @@
       </c>
       <c r="I1078" s="6" t="str">
         <f>VLOOKUP(F1078,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1079">
@@ -34552,7 +34552,7 @@
       </c>
       <c r="I1084" s="6" t="str">
         <f>VLOOKUP(F1084,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1085">
@@ -34645,7 +34645,7 @@
       </c>
       <c r="I1087" s="6" t="str">
         <f>VLOOKUP(F1087,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1088">
@@ -34769,7 +34769,7 @@
       </c>
       <c r="I1091" s="6" t="str">
         <f>VLOOKUP(F1091,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1092">
@@ -34893,7 +34893,7 @@
       </c>
       <c r="I1095" s="6" t="str">
         <f>VLOOKUP(F1095,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1096">
@@ -34986,7 +34986,7 @@
       </c>
       <c r="I1098" s="6" t="str">
         <f>VLOOKUP(F1098,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1099">
@@ -35079,7 +35079,7 @@
       </c>
       <c r="I1101" s="6" t="str">
         <f>VLOOKUP(F1101,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1102">
@@ -35234,7 +35234,7 @@
       </c>
       <c r="I1106" s="6" t="str">
         <f>VLOOKUP(F1106,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1107">
@@ -35296,7 +35296,7 @@
       </c>
       <c r="I1108" s="6" t="str">
         <f>VLOOKUP(F1108,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1109">
@@ -35389,7 +35389,7 @@
       </c>
       <c r="I1111" s="6" t="str">
         <f>VLOOKUP(F1111,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1112">
@@ -35544,7 +35544,7 @@
       </c>
       <c r="I1116" s="6" t="str">
         <f>VLOOKUP(F1116,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1117">
@@ -35668,7 +35668,7 @@
       </c>
       <c r="I1120" s="6" t="str">
         <f>VLOOKUP(F1120,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1121">
@@ -35823,7 +35823,7 @@
       </c>
       <c r="I1125" s="6" t="str">
         <f>VLOOKUP(F1125,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1126">
@@ -35916,7 +35916,7 @@
       </c>
       <c r="I1128" s="6" t="str">
         <f>VLOOKUP(F1128,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1129">
@@ -36040,7 +36040,7 @@
       </c>
       <c r="I1132" s="6" t="str">
         <f>VLOOKUP(F1132,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1133">
@@ -36195,7 +36195,7 @@
       </c>
       <c r="I1137" s="6" t="str">
         <f>VLOOKUP(F1137,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1138">
@@ -36350,7 +36350,7 @@
       </c>
       <c r="I1142" s="6" t="str">
         <f>VLOOKUP(F1142,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1143">
@@ -36412,7 +36412,7 @@
       </c>
       <c r="I1144" s="6" t="str">
         <f>VLOOKUP(F1144,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1145">
@@ -36474,7 +36474,7 @@
       </c>
       <c r="I1146" s="6" t="str">
         <f>VLOOKUP(F1146,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1147">
@@ -36536,7 +36536,7 @@
       </c>
       <c r="I1148" s="6" t="str">
         <f>VLOOKUP(F1148,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1149">
@@ -36598,7 +36598,7 @@
       </c>
       <c r="I1150" s="6" t="str">
         <f>VLOOKUP(F1150,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1151">
@@ -36660,7 +36660,7 @@
       </c>
       <c r="I1152" s="6" t="str">
         <f>VLOOKUP(F1152,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1153">
@@ -36722,7 +36722,7 @@
       </c>
       <c r="I1154" s="6" t="str">
         <f>VLOOKUP(F1154,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1155">
@@ -36815,7 +36815,7 @@
       </c>
       <c r="I1157" s="6" t="str">
         <f>VLOOKUP(F1157,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1158">
@@ -36908,7 +36908,7 @@
       </c>
       <c r="I1160" s="6" t="str">
         <f>VLOOKUP(F1160,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1161">
@@ -37001,7 +37001,7 @@
       </c>
       <c r="I1163" s="6" t="str">
         <f>VLOOKUP(F1163,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1164">
@@ -37094,7 +37094,7 @@
       </c>
       <c r="I1166" s="6" t="str">
         <f>VLOOKUP(F1166,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1167">
@@ -37218,7 +37218,7 @@
       </c>
       <c r="I1170" s="6" t="str">
         <f>VLOOKUP(F1170,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1171">
@@ -37342,7 +37342,7 @@
       </c>
       <c r="I1174" s="6" t="str">
         <f>VLOOKUP(F1174,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1175">
@@ -37435,7 +37435,7 @@
       </c>
       <c r="I1177" s="6" t="str">
         <f>VLOOKUP(F1177,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1178">
@@ -37497,7 +37497,7 @@
       </c>
       <c r="I1179" s="6" t="str">
         <f>VLOOKUP(F1179,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1180">
@@ -37621,7 +37621,7 @@
       </c>
       <c r="I1183" s="6" t="str">
         <f>VLOOKUP(F1183,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1184">
@@ -37745,7 +37745,7 @@
       </c>
       <c r="I1187" s="6" t="str">
         <f>VLOOKUP(F1187,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1188">
@@ -37838,7 +37838,7 @@
       </c>
       <c r="I1190" s="6" t="str">
         <f>VLOOKUP(F1190,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1191">
@@ -37931,7 +37931,7 @@
       </c>
       <c r="I1193" s="6" t="str">
         <f>VLOOKUP(F1193,lookups!$2:$110,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="1194">
@@ -45411,216 +45411,216 @@
         <v>105</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>109</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30">
@@ -45631,7 +45631,7 @@
         <v>148</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31">
@@ -45642,7 +45642,7 @@
         <v>150</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32">
@@ -45653,7 +45653,7 @@
         <v>152</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33">
@@ -45664,7 +45664,7 @@
         <v>154</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34">
@@ -45675,7 +45675,7 @@
         <v>156</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35">
@@ -45686,7 +45686,7 @@
         <v>158</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36">
@@ -45697,29 +45697,29 @@
         <v>160</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>163</v>
-      </c>
       <c r="C37" s="20" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="C38" s="20" t="s">
         <v>165</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="39">
@@ -45730,7 +45730,7 @@
         <v>167</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40">
@@ -45741,7 +45741,7 @@
         <v>169</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41">
@@ -45752,7 +45752,7 @@
         <v>171</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42">
@@ -45763,7 +45763,7 @@
         <v>173</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43">

</xml_diff>